<commit_message>
fine-tuned superblock code, nothing changed, am going to run the full scope of code
</commit_message>
<xml_diff>
--- a/outputs/df_superblocks.xlsx
+++ b/outputs/df_superblocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,1999 +612,2024 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[385, 412, 413, 407]</t>
+          <t>[376, 402, 373, 375]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[379, 405, 416, 419]</t>
+          <t>[397, 401, 405, 446]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>[384, 416, 417, 418, 419, 411, 405, 408, 379, 380, 381, 414]</t>
+          <t>[397, 400, 401, 370, 403, 372, 404, 374, 405, 381, 446, 447]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[379, 405, 416, 419]</t>
+          <t>[397, 401, 405, 446]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[416, 410, 387, 411]</t>
+          <t>[385, 412, 413, 407]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[354, 356, 383, 385]</t>
+          <t>[379, 405, 416, 419]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>[384, 385, 354, 355, 356, 386, 417, 409, 344, 345, 412, 383]</t>
+          <t>[384, 416, 417, 418, 419, 411, 405, 408, 379, 380, 381, 414]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[354, 356, 383, 385]</t>
+          <t>[379, 405, 416, 419]</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[418, 419, 413, 414]</t>
+          <t>[416, 410, 387, 411]</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[342, 356, 385, 452]</t>
+          <t>[354, 356, 383, 385]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>[385, 417, 356, 420, 452, 423, 424, 342, 407, 408, 412, 415]</t>
+          <t>[384, 385, 354, 355, 356, 386, 417, 409, 344, 345, 412, 383]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[342, 356, 385, 452]</t>
+          <t>[354, 356, 383, 385]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[426, 427, 430, 431]</t>
+          <t>[418, 419, 413, 414]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[356, 432, 452, 488]</t>
+          <t>[342, 356, 385, 452]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>[449, 356, 452, 423, 359, 361, 362, 424, 488, 432, 436, 477]</t>
+          <t>[385, 417, 356, 420, 452, 423, 424, 342, 407, 408, 412, 415]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[356, 432, 452, 488]</t>
+          <t>[342, 356, 385, 452]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[770, 789, 810, 773]</t>
+          <t>[426, 427, 430, 431]</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[767, 787, 794, 797]</t>
+          <t>[356, 432, 452, 488]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>[769, 772, 774, 811, 787, 788, 790, 794, 795, 796, 797, 767]</t>
+          <t>[449, 356, 452, 423, 359, 361, 362, 424, 488, 432, 436, 477]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[767, 787, 794, 797]</t>
+          <t>[356, 432, 452, 488]</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[804, 805, 798, 799]</t>
+          <t>[770, 789, 810, 773]</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[37, 457, 762, 797]</t>
+          <t>[767, 787, 794, 797]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>[803, 37, 806, 457, 458, 490, 812, 813, 816, 817, 762, 797]</t>
+          <t>[769, 772, 774, 811, 787, 788, 790, 794, 795, 796, 797, 767]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[37, 457, 762, 797]</t>
+          <t>[767, 787, 794, 797]</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[442, 443, 388, 389]</t>
+          <t>[804, 805, 798, 799]</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[349, 382, 785, 802]</t>
+          <t>[37, 457, 762, 797]</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>[800, 801, 802, 390, 392, 785, 406, 343, 444, 348, 349, 382]</t>
+          <t>[803, 37, 806, 457, 458, 490, 812, 813, 816, 817, 762, 797]</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[349, 382, 785, 802]</t>
+          <t>[37, 457, 762, 797]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[817, 805, 806, 799]</t>
+          <t>[442, 443, 388, 389]</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[458, 461, 766, 812]</t>
+          <t>[349, 382, 785, 802]</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>[804, 807, 457, 458, 490, 812, 461, 813, 798, 818, 762, 766]</t>
+          <t>[800, 801, 802, 390, 392, 785, 406, 343, 444, 348, 349, 382]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[458, 461, 766, 812]</t>
+          <t>[349, 382, 785, 802]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[444, 443, 348, 389]</t>
+          <t>[817, 805, 806, 799]</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>[390, 467, 800, 803]</t>
+          <t>[458, 461, 766, 812]</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>[800, 801, 802, 803, 388, 390, 392, 460, 467, 504, 442, 349]</t>
+          <t>[804, 807, 457, 458, 490, 812, 461, 813, 798, 818, 762, 766]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[390, 467, 800, 803]</t>
+          <t>[458, 461, 766, 812]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[731, 732, 685, 686]</t>
+          <t>[444, 443, 348, 389]</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[679, 681, 728, 736]</t>
+          <t>[390, 467, 800, 803]</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>[736, 737, 679, 680, 681, 684, 687, 660, 727, 728, 730, 733]</t>
+          <t>[800, 801, 802, 803, 388, 390, 392, 460, 467, 504, 442, 349]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[679, 681, 728, 736]</t>
+          <t>[390, 467, 800, 803]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[730, 731, 732, 733]</t>
+          <t>[731, 732, 685, 686]</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[684, 687, 688, 690]</t>
+          <t>[679, 681, 728, 736]</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>[736, 737, 684, 685, 686, 687, 688, 689, 690, 727, 728, 668]</t>
+          <t>[736, 737, 679, 680, 681, 684, 687, 660, 727, 728, 730, 733]</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[684, 687, 688, 690]</t>
+          <t>[679, 681, 728, 736]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[728, 724, 725, 727]</t>
+          <t>[730, 731, 732, 733]</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[554, 668, 669, 686]</t>
+          <t>[684, 687, 688, 690]</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>[554, 686, 590, 687, 690, 691, 722, 726, 730, 731, 668, 669]</t>
+          <t>[736, 737, 684, 685, 686, 687, 688, 689, 690, 727, 728, 668]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[554, 668, 669, 686]</t>
+          <t>[684, 687, 688, 690]</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[736, 737, 732, 733]</t>
+          <t>[728, 724, 725, 727]</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[667, 668, 683, 686]</t>
+          <t>[554, 668, 669, 686]</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>[738, 739, 683, 684, 685, 686, 688, 689, 730, 667, 668, 731]</t>
+          <t>[554, 686, 590, 687, 690, 691, 722, 726, 730, 731, 668, 669]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[667, 668, 686]</t>
+          <t>[554, 668, 669, 686]</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[728, 730, 731, 727]</t>
+          <t>[736, 737, 732, 733]</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[685, 689, 691, 726]</t>
+          <t>[667, 668, 683, 686]</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>[732, 685, 686, 687, 689, 690, 691, 724, 725, 726, 668, 733]</t>
+          <t>[738, 739, 683, 684, 685, 686, 688, 689, 730, 667, 668, 731]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[685, 689, 691, 726]</t>
+          <t>[667, 668, 683, 686]</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[754, 753, 746, 747]</t>
+          <t>[728, 730, 731, 727]</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>[656, 672, 696, 698]</t>
+          <t>[685, 689, 691, 726]</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[672, 647, 745, 748, 656, 752, 723, 755, 661, 696, 697, 698]</t>
+          <t>[732, 685, 686, 687, 689, 690, 691, 724, 725, 726, 668, 733]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[656, 672, 696, 698]</t>
+          <t>[685, 689, 691, 726]</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[695, 691, 669, 663]</t>
+          <t>[754, 753, 746, 747]</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>[696, 698, 721, 728]</t>
+          <t>[656, 672, 696, 698]</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[728, 721, 690, 722, 723, 724, 694, 696, 697, 698, 670, 671]</t>
+          <t>[672, 647, 745, 748, 656, 752, 723, 755, 661, 696, 697, 698]</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[696, 698, 721, 728]</t>
+          <t>[656, 672, 696, 698]</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[690, 691, 694, 695]</t>
+          <t>[695, 691, 669, 663]</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[697, 722, 729, 730]</t>
+          <t>[696, 698, 721, 728]</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>[728, 722, 723, 724, 729, 662, 663, 696, 697, 730, 668, 669]</t>
+          <t>[728, 721, 690, 722, 723, 724, 694, 696, 697, 698, 670, 671]</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>[697, 722, 729, 730]</t>
+          <t>[696, 698, 721, 728]</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[515, 498, 514, 500]</t>
+          <t>[690, 691, 694, 695]</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>[450, 454, 476, 502]</t>
+          <t>[697, 722, 729, 730]</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>[513, 450, 503, 516, 454, 455, 462, 497, 502, 471, 472, 476]</t>
+          <t>[728, 722, 723, 724, 729, 662, 663, 696, 697, 730, 668, 669]</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[450, 454, 476, 502]</t>
+          <t>[697, 722, 729, 730]</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[496, 497, 512, 513]</t>
+          <t>[515, 498, 514, 500]</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[451, 453, 455, 462]</t>
+          <t>[450, 454, 476, 502]</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>[450, 451, 514, 453, 454, 455, 492, 462, 495, 498, 475, 511]</t>
+          <t>[513, 450, 503, 516, 454, 455, 462, 497, 502, 471, 472, 476]</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[451, 453, 455, 462]</t>
+          <t>[450, 454, 476, 502]</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[564, 565, 502, 510]</t>
+          <t>[496, 497, 512, 513]</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>[473, 500, 528, 549]</t>
+          <t>[451, 453, 455, 462]</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>[548, 549, 528, 529, 563, 500, 501, 566, 503, 472, 473, 509]</t>
+          <t>[450, 451, 514, 453, 454, 455, 492, 462, 495, 498, 475, 511]</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[473, 500, 528, 549]</t>
+          <t>[451, 453, 455, 462]</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[529, 548, 565, 564]</t>
+          <t>[564, 565, 502, 510]</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>[501, 503, 521, 552]</t>
+          <t>[473, 500, 528, 549]</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>[549, 551, 552, 521, 522, 528, 563, 501, 502, 503, 566, 510]</t>
+          <t>[548, 549, 528, 529, 563, 500, 501, 566, 503, 472, 473, 509]</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[501, 503, 521, 552]</t>
+          <t>[473, 500, 528, 549]</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[472, 508, 509, 462]</t>
+          <t>[529, 548, 565, 564]</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>[457, 497, 501, 503]</t>
+          <t>[501, 503, 521, 552]</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>[450, 457, 461, 497, 498, 500, 501, 502, 503, 473, 507, 510]</t>
+          <t>[549, 551, 552, 521, 522, 528, 563, 501, 502, 503, 566, 510]</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[457, 497, 501, 503]</t>
+          <t>[501, 503, 521, 552]</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[566, 549, 550, 567]</t>
+          <t>[472, 508, 509, 462]</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>[476, 502, 522, 523]</t>
+          <t>[457, 497, 501, 503]</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>[516, 552, 553, 522, 523, 529, 530, 565, 502, 503, 568, 476]</t>
+          <t>[450, 457, 461, 497, 498, 500, 501, 502, 503, 473, 507, 510]</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[476, 502, 522, 523]</t>
+          <t>[457, 497, 501, 503]</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[560, 582, 558, 583]</t>
+          <t>[566, 549, 550, 567]</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>[522, 523, 540, 588]</t>
+          <t>[476, 502, 522, 523]</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>[580, 581, 552, 553, 522, 523, 584, 557, 587, 559, 588, 540]</t>
+          <t>[516, 552, 553, 522, 523, 529, 530, 565, 502, 503, 568, 476]</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[522, 523, 540, 588]</t>
+          <t>[476, 502, 522, 523]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[576, 577, 534, 542]</t>
+          <t>[560, 582, 558, 583]</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>[240, 530, 572, 580]</t>
+          <t>[522, 523, 540, 588]</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>[578, 573, 580, 581, 523, 239, 240, 530, 531, 572, 541, 575]</t>
+          <t>[580, 581, 552, 553, 522, 523, 584, 557, 587, 559, 588, 540]</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>[240, 530, 580]</t>
+          <t>[522, 523, 540, 588]</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[552, 553, 558, 582]</t>
+          <t>[576, 577, 534, 542]</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>[529, 530, 559, 580]</t>
+          <t>[240, 530, 572, 580]</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>[580, 549, 550, 581, 583, 522, 523, 557, 559, 560, 529, 530]</t>
+          <t>[578, 573, 580, 581, 523, 239, 240, 530, 531, 572, 541, 575]</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[529, 530, 559, 580]</t>
+          <t>[240, 530, 572, 580]</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[569, 482, 570, 485]</t>
+          <t>[552, 553, 558, 582]</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>[471, 526, 530, 572]</t>
+          <t>[529, 530, 559, 580]</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>[481, 546, 526, 530, 531, 470, 471, 568, 571, 476, 541, 572]</t>
+          <t>[580, 549, 550, 581, 583, 522, 523, 557, 559, 560, 529, 530]</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[471, 526, 530]</t>
+          <t>[529, 530, 559, 580]</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[560, 557, 558, 559]</t>
+          <t>[569, 482, 570, 485]</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>[551, 553, 584, 589]</t>
+          <t>[471, 526, 530, 572]</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>[582, 551, 552, 553, 522, 583, 556, 584, 587, 588, 589, 535]</t>
+          <t>[481, 546, 526, 530, 531, 470, 471, 568, 571, 476, 541, 572]</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[551, 553, 584, 589]</t>
+          <t>[471, 526, 530, 572]</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[529, 565, 549, 566]</t>
+          <t>[560, 557, 558, 559]</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>[510, 516, 551, 553]</t>
+          <t>[551, 553, 584, 589]</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>[516, 548, 550, 551, 552, 553, 522, 567, 564, 502, 503, 510]</t>
+          <t>[582, 551, 552, 553, 522, 583, 556, 584, 587, 588, 589, 535]</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>[510, 516, 551, 553]</t>
+          <t>[551, 553, 584, 589]</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[744, 743, 734, 735]</t>
+          <t>[529, 565, 549, 566]</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[651, 662, 700, 751]</t>
+          <t>[510, 516, 551, 553]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>[740, 742, 651, 751, 692, 693, 662, 729, 700, 701, 702, 703]</t>
+          <t>[516, 548, 550, 551, 552, 553, 522, 567, 564, 502, 503, 510]</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[662, 700, 751]</t>
+          <t>[510, 516, 551, 553]</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[656, 752, 753, 647]</t>
+          <t>[744, 743, 734, 735]</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[703, 708, 710, 747]</t>
+          <t>[651, 662, 700, 751]</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>[708, 709, 710, 648, 745, 746, 747, 654, 751, 754, 661, 703]</t>
+          <t>[740, 742, 651, 751, 692, 693, 662, 729, 700, 701, 702, 703]</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[703, 708, 710, 747]</t>
+          <t>[651, 662, 700, 751]</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[671, 669, 670, 663]</t>
+          <t>[656, 752, 753, 647]</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>[589, 699, 723, 724]</t>
+          <t>[703, 708, 710, 747]</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>[589, 657, 721, 691, 722, 723, 724, 695, 536, 697, 698, 699]</t>
+          <t>[708, 709, 710, 648, 745, 746, 747, 654, 751, 754, 661, 703]</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[589, 699, 723, 724]</t>
+          <t>[703, 708, 710, 747]</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[754, 747, 748, 755]</t>
+          <t>[671, 669, 670, 663]</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>[647, 658, 699, 723]</t>
+          <t>[589, 699, 723, 724]</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>[672, 647, 746, 749, 753, 658, 723, 756, 661, 697, 698, 699]</t>
+          <t>[589, 657, 721, 691, 722, 723, 724, 695, 536, 697, 698, 699]</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[647, 658, 699, 723]</t>
+          <t>[589, 699, 723, 724]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[672, 754, 755, 661]</t>
+          <t>[754, 747, 748, 755]</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>[648, 714, 746, 749]</t>
+          <t>[647, 658, 699, 723]</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>[710, 711, 648, 647, 714, 746, 747, 748, 749, 753, 658, 756]</t>
+          <t>[672, 647, 746, 749, 753, 658, 723, 756, 661, 697, 698, 699]</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[714, 746, 749]</t>
+          <t>[647, 658, 699, 723]</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[544, 537, 540, 543]</t>
+          <t>[672, 754, 755, 661]</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>[53, 539, 575, 583]</t>
+          <t>[648, 714, 746, 749]</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>[578, 579, 580, 583, 584, 585, 525, 53, 538, 539, 574, 575]</t>
+          <t>[710, 711, 648, 647, 714, 746, 747, 748, 749, 753, 658, 756]</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[53, 539, 575, 583]</t>
+          <t>[648, 714, 746, 749]</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[497, 498, 514, 513]</t>
+          <t>[544, 537, 540, 543]</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>[471, 472, 475, 492]</t>
+          <t>[53, 539, 575, 583]</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>[512, 450, 515, 454, 455, 492, 462, 496, 500, 471, 472, 475]</t>
+          <t>[578, 579, 580, 583, 584, 585, 525, 53, 538, 539, 574, 575]</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[471, 472, 475, 492]</t>
+          <t>[53, 539, 575, 583]</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[544, 537, 540, 543]</t>
+          <t>[497, 498, 514, 513]</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>[539, 575, 583, 586]</t>
+          <t>[471, 472, 475, 492]</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>[578, 579, 580, 583, 584, 585, 586, 525, 538, 539, 574, 575]</t>
+          <t>[512, 450, 515, 454, 455, 492, 462, 496, 500, 471, 472, 475]</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[539, 575, 583, 586]</t>
+          <t>[471, 472, 475, 492]</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[531, 541, 534, 542]</t>
+          <t>[544, 537, 540, 543]</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>[239, 568, 571, 581]</t>
+          <t>[539, 575, 583, 586]</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>[576, 577, 581, 523, 239, 530, 568, 569, 570, 571, 572, 573]</t>
+          <t>[578, 579, 580, 583, 584, 585, 586, 525, 538, 539, 574, 575]</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[239, 568, 571, 581]</t>
+          <t>[539, 575, 583, 586]</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[576, 577, 578, 575]</t>
+          <t>[531, 541, 534, 542]</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>[241, 523, 540, 573]</t>
+          <t>[239, 568, 571, 581]</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>[580, 581, 574, 523, 239, 240, 241, 534, 540, 573, 542, 543]</t>
+          <t>[576, 577, 581, 523, 239, 530, 568, 569, 570, 571, 572, 573]</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[523, 540, 573]</t>
+          <t>[239, 568, 571, 581]</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[577, 578, 580, 581]</t>
+          <t>[576, 577, 578, 575]</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>[534, 553, 574, 584]</t>
+          <t>[241, 523, 540, 573]</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>[576, 582, 583, 574, 553, 584, 523, 575, 534, 540, 542, 543]</t>
+          <t>[580, 581, 574, 523, 239, 240, 241, 534, 540, 573, 542, 543]</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[534, 553, 574, 584]</t>
+          <t>[241, 523, 540, 573]</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[408, 413, 414, 407]</t>
+          <t>[577, 578, 580, 581]</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>[380, 382, 417, 420]</t>
+          <t>[534, 553, 574, 584]</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>[385, 417, 418, 419, 420, 405, 342, 412, 380, 381, 382, 415]</t>
+          <t>[576, 582, 583, 574, 553, 584, 523, 575, 534, 540, 542, 543]</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[380, 382, 417, 420]</t>
+          <t>[534, 553, 574, 584]</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[416, 417, 411, 412]</t>
+          <t>[408, 413, 414, 407]</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>[344, 345, 407, 423]</t>
+          <t>[380, 382, 417, 420]</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>[384, 385, 418, 355, 356, 387, 423, 407, 344, 345, 410, 413]</t>
+          <t>[385, 417, 418, 419, 420, 405, 342, 412, 380, 381, 382, 415]</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[344, 345, 407, 423]</t>
+          <t>[380, 382, 417, 420]</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[384, 385, 411, 412]</t>
+          <t>[416, 417, 411, 412]</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>[378, 381, 387, 418]</t>
+          <t>[344, 345, 407, 423]</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>[416, 417, 418, 387, 410, 407, 344, 378, 379, 380, 381, 413]</t>
+          <t>[384, 385, 418, 355, 356, 387, 423, 407, 344, 345, 410, 413]</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[378, 381, 387, 418]</t>
+          <t>[344, 345, 407, 423]</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[344, 410, 411, 384]</t>
+          <t>[384, 385, 411, 412]</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>[377, 380, 386, 417]</t>
+          <t>[378, 381, 387, 418]</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>[416, 385, 386, 387, 417, 409, 377, 378, 379, 380, 412, 383]</t>
+          <t>[416, 417, 418, 387, 410, 407, 344, 378, 379, 380, 381, 413]</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[380, 386, 417]</t>
+          <t>[378, 381, 387, 418]</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[785, 403, 404, 343]</t>
+          <t>[344, 410, 411, 384]</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>[381, 400, 442, 809]</t>
+          <t>[377, 380, 386, 417]</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[800, 388, 808, 809, 400, 401, 402, 405, 406, 376, 442, 381]</t>
+          <t>[416, 385, 386, 387, 417, 409, 377, 378, 379, 380, 412, 383]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[381, 400, 442, 809]</t>
+          <t>[377, 380, 386, 417]</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[376, 402, 403, 404]</t>
+          <t>[785, 403, 404, 343]</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>[370, 406, 447, 808]</t>
+          <t>[381, 400, 442, 809]</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[808, 400, 401, 370, 785, 373, 405, 375, 406, 381, 343, 447]</t>
+          <t>[800, 388, 808, 809, 400, 401, 402, 405, 406, 376, 442, 381]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[370, 406, 447, 808]</t>
+          <t>[381, 400, 442, 809]</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[408, 414, 342, 415]</t>
+          <t>[376, 402, 403, 404]</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>[381, 390, 418, 421]</t>
+          <t>[370, 406, 447, 808]</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>[418, 419, 420, 421, 390, 391, 393, 413, 405, 407, 381, 382]</t>
+          <t>[808, 400, 401, 370, 785, 373, 405, 375, 406, 381, 343, 447]</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>[381, 390, 418, 421]</t>
+          <t>[370, 406, 447, 808]</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[457, 507, 508, 461]</t>
+          <t>[408, 414, 342, 415]</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>[472, 492, 805, 819]</t>
+          <t>[381, 390, 418, 421]</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>[450, 805, 806, 807, 490, 492, 462, 819, 472, 473, 506, 509]</t>
+          <t>[418, 419, 420, 421, 390, 391, 393, 413, 405, 407, 381, 382]</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[472, 492, 805, 819]</t>
+          <t>[381, 390, 418, 421]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[472, 498, 500, 462]</t>
+          <t>[457, 507, 508, 461]</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>[507, 510, 513, 516]</t>
+          <t>[472, 492, 805, 819]</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>[513, 450, 514, 515, 516, 497, 502, 503, 507, 508, 509, 510]</t>
+          <t>[450, 805, 806, 807, 490, 492, 462, 819, 472, 473, 506, 509]</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>[507, 510, 513, 516]</t>
+          <t>[472, 492, 805, 819]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[457, 490, 506, 507]</t>
+          <t>[472, 498, 500, 462]</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>[451, 462, 804, 807]</t>
+          <t>[507, 510, 513, 516]</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>[450, 451, 804, 805, 806, 807, 458, 492, 461, 462, 505, 508]</t>
+          <t>[513, 450, 514, 515, 516, 497, 502, 503, 507, 508, 509, 510]</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>[451, 462, 804, 807]</t>
+          <t>[507, 510, 513, 516]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[515, 476, 516, 471]</t>
+          <t>[457, 490, 506, 507]</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>[498, 520, 566, 569]</t>
+          <t>[451, 462, 804, 807]</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>[481, 482, 514, 567, 455, 520, 498, 500, 566, 503, 568, 569]</t>
+          <t>[450, 451, 804, 805, 806, 807, 458, 492, 461, 462, 505, 508]</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[498, 566, 569]</t>
+          <t>[451, 462, 804, 807]</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[804, 805, 798, 799]</t>
+          <t>[515, 476, 516, 471]</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>[457, 460, 762, 797]</t>
+          <t>[498, 520, 566, 569]</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>[803, 806, 457, 458, 490, 460, 812, 813, 816, 817, 762, 797]</t>
+          <t>[481, 482, 514, 567, 455, 520, 498, 500, 566, 503, 568, 569]</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>[457, 460, 762, 797]</t>
+          <t>[498, 520, 566, 569]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[457, 490, 805, 806]</t>
+          <t>[804, 805, 798, 799]</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>[505, 508, 798, 818]</t>
+          <t>[457, 460, 762, 797]</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>[804, 807, 458, 461, 817, 818, 505, 506, 507, 508, 798, 799]</t>
+          <t>[803, 806, 457, 458, 490, 460, 812, 813, 816, 817, 762, 797]</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>[505, 508, 798, 818]</t>
+          <t>[457, 460, 762, 797]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[472, 509, 502, 510]</t>
+          <t>[457, 490, 805, 806]</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>[461, 498, 563, 566]</t>
+          <t>[505, 508, 798, 818]</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>[461, 462, 498, 563, 500, 501, 564, 503, 565, 473, 566, 508]</t>
+          <t>[804, 807, 458, 461, 817, 818, 505, 506, 507, 508, 798, 799]</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[461, 498, 563, 566]</t>
+          <t>[505, 508, 798, 818]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[481, 482, 476, 471]</t>
+          <t>[472, 509, 502, 510]</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>[463, 514, 567, 570]</t>
+          <t>[461, 498, 563, 566]</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>[514, 515, 516, 485, 455, 520, 463, 470, 567, 568, 569, 570]</t>
+          <t>[461, 462, 498, 563, 500, 501, 564, 503, 565, 473, 566, 508]</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>[463, 514, 567, 570]</t>
+          <t>[461, 498, 563, 566]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[568, 569, 482, 476]</t>
+          <t>[481, 482, 476, 471]</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>[470, 515, 531, 550]</t>
+          <t>[463, 514, 567, 570]</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>[481, 515, 516, 485, 550, 567, 530, 531, 470, 471, 570, 541]</t>
+          <t>[514, 515, 516, 485, 455, 520, 463, 470, 567, 568, 569, 570]</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>[470, 515, 531, 550]</t>
+          <t>[463, 514, 567, 570]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[568, 476, 516, 567]</t>
+          <t>[568, 569, 482, 476]</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>[481, 500, 541, 549]</t>
+          <t>[470, 515, 531, 550]</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>[481, 482, 471, 515, 549, 550, 530, 500, 566, 503, 569, 541]</t>
+          <t>[481, 515, 516, 485, 550, 567, 530, 531, 470, 471, 570, 541]</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[481, 500, 541, 549]</t>
+          <t>[470, 515, 531, 550]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[569, 570, 531, 541]</t>
+          <t>[568, 476, 516, 567]</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>[476, 523, 546, 573]</t>
+          <t>[481, 500, 541, 549]</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>[482, 546, 485, 523, 530, 534, 572, 568, 571, 476, 573, 542]</t>
+          <t>[481, 482, 471, 515, 549, 550, 530, 500, 566, 503, 569, 541]</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>[476, 523, 546, 573]</t>
+          <t>[481, 500, 541, 549]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[457, 461, 806, 807]</t>
+          <t>[569, 570, 531, 541]</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>[506, 509, 777, 799]</t>
+          <t>[476, 523, 546, 573]</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>[805, 777, 490, 817, 818, 819, 473, 506, 507, 508, 509, 799]</t>
+          <t>[482, 546, 485, 523, 530, 534, 572, 568, 571, 476, 573, 542]</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>[506, 509, 777, 799]</t>
+          <t>[476, 523, 546, 573]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[552, 553, 549, 550]</t>
+          <t>[457, 461, 806, 807]</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>[557, 565, 568, 581]</t>
+          <t>[506, 509, 777, 799]</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>[581, 582, 522, 523, 557, 558, 529, 530, 565, 566, 567, 568]</t>
+          <t>[805, 777, 490, 817, 818, 819, 473, 506, 507, 508, 509, 799]</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[557, 565, 568, 581]</t>
+          <t>[506, 509, 777, 799]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[580, 581, 582, 583]</t>
+          <t>[552, 553, 549, 550]</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>[542, 543, 552, 587]</t>
+          <t>[557, 565, 568, 581]</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>[577, 578, 552, 553, 584, 523, 587, 558, 560, 540, 542, 543]</t>
+          <t>[581, 582, 522, 523, 557, 558, 529, 530, 565, 566, 567, 568]</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>[542, 543, 552, 587]</t>
+          <t>[557, 565, 568, 581]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[560, 587, 584, 583]</t>
+          <t>[580, 581, 582, 583]</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>[536, 537, 557, 581]</t>
+          <t>[542, 543, 552, 587]</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>[580, 581, 582, 585, 588, 557, 558, 559, 561, 536, 537, 540]</t>
+          <t>[577, 578, 552, 553, 584, 523, 587, 558, 560, 540, 542, 543]</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>[536, 537, 557, 581]</t>
+          <t>[542, 543, 552, 587]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[671, 697, 698, 663]</t>
+          <t>[560, 587, 584, 583]</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>[536, 691, 746, 749]</t>
+          <t>[536, 537, 557, 581]</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>[746, 747, 748, 749, 657, 691, 723, 695, 536, 699, 669, 670]</t>
+          <t>[580, 581, 582, 585, 588, 557, 558, 559, 561, 536, 537, 540]</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[536, 691, 746, 749]</t>
+          <t>[536, 537, 557, 581]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[697, 698, 747, 748]</t>
+          <t>[671, 697, 698, 663]</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>[657, 695, 753, 756]</t>
+          <t>[536, 691, 746, 749]</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>[663, 746, 749, 657, 753, 723, 754, 755, 756, 695, 699, 671]</t>
+          <t>[746, 747, 748, 749, 657, 691, 723, 695, 536, 699, 669, 670]</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>[657, 695, 753, 756]</t>
+          <t>[536, 691, 746, 749]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[756, 755, 748, 749]</t>
+          <t>[697, 698, 747, 748]</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>[661, 673, 697, 705]</t>
+          <t>[657, 695, 753, 756]</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>[672, 673, 705, 747, 750, 658, 754, 661, 757, 697, 698, 699]</t>
+          <t>[663, 746, 749, 657, 753, 723, 754, 755, 756, 695, 699, 671]</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>[661, 673, 697]</t>
+          <t>[657, 695, 753, 756]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[553, 523, 581, 582]</t>
+          <t>[756, 755, 748, 749]</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>[541, 549, 560, 578]</t>
+          <t>[661, 673, 697, 705]</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>[577, 578, 580, 549, 550, 583, 552, 558, 560, 530, 541, 542]</t>
+          <t>[672, 673, 705, 747, 750, 658, 754, 661, 757, 697, 698, 699]</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[541, 549, 560, 578]</t>
+          <t>[661, 673, 697, 705]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[577, 523, 581, 542]</t>
+          <t>[553, 523, 581, 582]</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>[531, 550, 575, 583]</t>
+          <t>[541, 549, 560, 578]</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>[576, 578, 580, 550, 582, 583, 553, 530, 531, 534, 541, 575]</t>
+          <t>[577, 578, 580, 549, 550, 583, 552, 558, 560, 530, 541, 542]</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>[531, 550, 575, 583]</t>
+          <t>[541, 549, 560, 578]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[584, 540, 583, 580]</t>
+          <t>[577, 523, 581, 542]</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>[544, 558, 561, 577]</t>
+          <t>[531, 550, 575, 583]</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>[544, 577, 578, 581, 582, 585, 587, 558, 560, 561, 537, 543]</t>
+          <t>[576, 578, 580, 550, 582, 583, 553, 530, 531, 534, 541, 575]</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>[544, 558, 561, 577]</t>
+          <t>[531, 550, 575, 583]</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[728, 690, 691, 724]</t>
+          <t>[584, 540, 583, 580]</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>[590, 662, 663, 731]</t>
+          <t>[544, 558, 561, 577]</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>[695, 727, 590, 722, 725, 662, 663, 694, 730, 731, 668, 669]</t>
+          <t>[544, 577, 578, 581, 582, 585, 587, 558, 560, 561, 537, 543]</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[590, 662, 663, 731]</t>
+          <t>[544, 558, 561, 577]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[737, 732, 684, 685]</t>
+          <t>[728, 690, 691, 724]</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>[649, 660, 730, 739]</t>
+          <t>[590, 662, 663, 731]</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>[736, 738, 739, 679, 680, 649, 683, 686, 660, 730, 731, 733]</t>
+          <t>[695, 727, 590, 722, 725, 662, 663, 694, 730, 731, 668, 669]</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>[649, 660, 730]</t>
+          <t>[590, 662, 663, 731]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[692, 693, 734, 735]</t>
+          <t>[737, 732, 684, 685]</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>[667, 668, 703, 742]</t>
+          <t>[649, 660, 730, 739]</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>[740, 742, 743, 744, 651, 688, 689, 662, 729, 667, 668, 703]</t>
+          <t>[736, 738, 739, 679, 680, 649, 683, 686, 660, 730, 731, 733]</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>[667, 668, 703, 742]</t>
+          <t>[649, 660, 730, 739]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[752, 745, 751, 703]</t>
+          <t>[692, 693, 734, 735]</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>[647, 704, 723, 734]</t>
+          <t>[667, 668, 703, 742]</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>[704, 647, 744, 746, 734, 654, 656, 753, 723, 696, 729, 702]</t>
+          <t>[740, 742, 743, 744, 651, 688, 689, 662, 729, 667, 668, 703]</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[647, 704, 723, 734]</t>
+          <t>[667, 668, 703, 742]</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[656, 752, 654, 751]</t>
+          <t>[752, 745, 751, 703]</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>[648, 707, 744, 746]</t>
+          <t>[647, 704, 723, 734]</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>[704, 707, 708, 709, 647, 648, 744, 745, 746, 753, 702, 703]</t>
+          <t>[704, 647, 744, 746, 734, 654, 656, 753, 723, 696, 729, 702]</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>[707, 744, 746]</t>
+          <t>[647, 704, 723, 734]</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[744, 729, 734, 703]</t>
+          <t>[656, 752, 654, 751]</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>[692, 694, 701, 752]</t>
+          <t>[648, 707, 744, 746]</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>[743, 745, 751, 752, 692, 693, 694, 662, 696, 701, 702, 735]</t>
+          <t>[704, 707, 708, 709, 647, 648, 744, 745, 746, 753, 702, 703]</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>[692, 694, 701, 752]</t>
+          <t>[648, 707, 744, 746]</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[752, 745, 746, 753]</t>
+          <t>[744, 729, 734, 703]</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>[654, 661, 697, 729]</t>
+          <t>[692, 694, 701, 752]</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>[647, 747, 654, 751, 656, 754, 723, 729, 661, 696, 697, 703]</t>
+          <t>[743, 745, 751, 752, 692, 693, 694, 662, 696, 701, 702, 735]</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>[654, 661, 697, 729]</t>
+          <t>[692, 694, 701, 752]</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[753, 754, 661, 647]</t>
+          <t>[752, 745, 746, 753]</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>[709, 711, 745, 748]</t>
+          <t>[654, 661, 697, 729]</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>[672, 709, 710, 711, 648, 745, 746, 747, 748, 656, 752, 755]</t>
+          <t>[647, 747, 654, 751, 656, 754, 723, 729, 661, 696, 697, 703]</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>[709, 745, 748]</t>
+          <t>[654, 661, 697, 729]</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[697, 746, 723, 747]</t>
+          <t>[753, 754, 661, 647]</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>[671, 694, 752, 755]</t>
+          <t>[709, 711, 745, 748]</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>[663, 745, 748, 752, 753, 754, 755, 694, 695, 696, 698, 671]</t>
+          <t>[672, 709, 710, 711, 648, 745, 746, 747, 748, 656, 752, 755]</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>[671, 694, 752, 755]</t>
+          <t>[709, 711, 745, 748]</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[680, 660, 685, 686]</t>
+          <t>[697, 746, 723, 747]</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>[677, 678, 727, 737]</t>
+          <t>[671, 694, 752, 755]</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>[737, 677, 678, 679, 741, 681, 684, 687, 727, 666, 731, 732]</t>
+          <t>[663, 745, 748, 752, 753, 754, 755, 694, 695, 696, 698, 671]</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>[678, 727, 737]</t>
+          <t>[671, 694, 752, 755]</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[729, 734, 693, 662]</t>
+          <t>[680, 660, 685, 686]</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>[688, 690, 743, 745]</t>
+          <t>[677, 678, 727, 737]</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>[743, 744, 745, 688, 689, 690, 735, 692, 694, 696, 668, 703]</t>
+          <t>[737, 677, 678, 679, 741, 681, 684, 687, 727, 666, 731, 732]</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>[688, 690, 743, 745]</t>
+          <t>[677, 678, 727, 737]</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>[729, 734, 693, 662]</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>[688, 690, 743, 745]</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>[743, 744, 745, 688, 689, 690, 735, 692, 694, 696, 668, 703]</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>[688, 690, 743, 745]</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
         <v>86</v>
       </c>
-      <c r="B87" t="inlineStr">
+      <c r="B88" t="inlineStr">
         <is>
           <t>[695, 697, 723, 663]</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t>[670, 690, 745, 748]</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr">
+      <c r="D88" t="inlineStr">
         <is>
           <t>[745, 746, 747, 748, 690, 691, 694, 696, 698, 669, 670, 671]</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr">
+      <c r="E88" t="inlineStr">
         <is>
           <t>[670, 690, 745, 748]</t>
         </is>

</xml_diff>